<commit_message>
Feat: crawling daum movies
</commit_message>
<xml_diff>
--- a/xlsx/data.xlsx
+++ b/xlsx/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zerocho\WebstormProjects\nodejs-crawler\lecture\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grs04\Desktop\project\node-crawler\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D534095-73C5-41F8-B748-B82DB9D03CD9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7017991F-7E6E-4AB5-8D81-B0253AD27EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="영화목록" sheetId="1" r:id="rId1"/>
@@ -22,87 +22,74 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
-    <t>https://movie.naver.com/movie/bi/mi/basic.nhn?code=24452</t>
-  </si>
-  <si>
-    <t>https://movie.naver.com/movie/bi/mi/basic.nhn?code=31794</t>
-  </si>
-  <si>
-    <t>https://movie.naver.com/movie/bi/mi/basic.nhn?code=72363</t>
-  </si>
-  <si>
-    <t>https://movie.naver.com/movie/bi/mi/basic.nhn?code=100931</t>
-  </si>
-  <si>
-    <t>https://movie.naver.com/movie/bi/mi/basic.nhn?code=30688</t>
-  </si>
-  <si>
-    <t>타이타닉</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>아바타</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>매트릭스</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>반지의 제왕</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>어벤져스</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>겨울왕국</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>트랜스포머</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>해리 포터</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>다크나이트</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>캐리비안의 해적</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://movie.naver.com/movie/bi/mi/basic.nhn?code=62586</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://movie.naver.com/movie/bi/mi/basic.nhn?code=37148</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://movie.naver.com/movie/bi/mi/basic.nhn?code=62266</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://movie.naver.com/movie/bi/mi/basic.nhn?code=18847</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://movie.naver.com/movie/bi/mi/basic.nhn?code=61521</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>제목</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
     <t>링크</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>미션 임파서블: 데드 레코닝 PART ONE</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://movie.daum.net/moviedb/main?movieId=139236</t>
+  </si>
+  <si>
+    <t>https://movie.daum.net/moviedb/main?movieId=163777</t>
+  </si>
+  <si>
+    <t>https://movie.daum.net/moviedb/main?movieId=62731</t>
+  </si>
+  <si>
+    <t>인디아나 존스: 운명의 다이얼</t>
+  </si>
+  <si>
+    <t>엘리멘탈</t>
+  </si>
+  <si>
+    <t>https://movie.daum.net/moviedb/main?movieId=136532</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>스파이더맨: 어크로스 더 유니버스</t>
+  </si>
+  <si>
+    <t>악마들</t>
+  </si>
+  <si>
+    <t>https://movie.daum.net/moviedb/main?movieId=158891</t>
+  </si>
+  <si>
+    <t>범죄도시3</t>
+  </si>
+  <si>
+    <t>https://movie.daum.net/moviedb/main?movieId=160244</t>
+  </si>
+  <si>
+    <t>귀공자</t>
+  </si>
+  <si>
+    <t>https://movie.daum.net/moviedb/main?movieId=155850</t>
+  </si>
+  <si>
+    <t>여름날 우리</t>
+  </si>
+  <si>
+    <t>https://movie.daum.net/moviedb/main?movieId=151333</t>
+  </si>
+  <si>
+    <t>https://movie.daum.net/moviedb/main?movieId=150228</t>
+  </si>
+  <si>
+    <t>기적을 믿는 소녀</t>
+  </si>
+  <si>
+    <t>수라</t>
+  </si>
+  <si>
+    <t>https://movie.daum.net/moviedb/main?movieId=163796</t>
   </si>
 </sst>
 </file>
@@ -1073,7 +1060,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1084,100 +1071,96 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B11" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="B8" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B5" r:id="rId1" xr:uid="{7326113D-2188-4CB8-91A5-C708107049E6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>